<commit_message>
c rev with zip
</commit_message>
<xml_diff>
--- a/ComparedResults/DIV2_Tables.xlsx
+++ b/ComparedResults/DIV2_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neild\Desktop\DIV2 Payroll Analysis\ComparedResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11A52CF-4791-41E6-B8BB-8AF027FA441D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB0D3EF-6F75-4072-AEFC-30C8F1C608F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1236,8 +1236,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="2" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1245,10 +1244,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1259,13 +1258,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="2">
-        <v>566.66</v>
+        <v>2641.24</v>
       </c>
       <c r="C2" s="2">
-        <v>1631.5</v>
+        <v>1152.02</v>
       </c>
       <c r="D2" s="4">
-        <v>-1064.8399999999999</v>
+        <v>-1489.22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1273,13 +1272,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>6639</v>
+        <v>13278.34</v>
       </c>
       <c r="C3" s="2">
-        <v>5817.16</v>
+        <v>13893.26</v>
       </c>
       <c r="D3" s="3">
-        <v>821.83</v>
+        <v>614.91999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1287,13 +1286,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>1245.8499999999999</v>
+        <v>2024.62</v>
       </c>
       <c r="C4" s="2">
-        <v>1239.97</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5.88</v>
+        <v>1852.16</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-172.46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1301,13 +1300,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>7408.82</v>
+        <v>13231.05</v>
       </c>
       <c r="C5" s="2">
-        <v>6077.61</v>
+        <v>14843.35</v>
       </c>
       <c r="D5" s="3">
-        <v>1331.21</v>
+        <v>1612.3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1315,13 +1314,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>2548.19</v>
+        <v>4626.1000000000004</v>
       </c>
       <c r="C6" s="2">
-        <v>3422</v>
-      </c>
-      <c r="D6" s="4">
-        <v>-873.8</v>
+        <v>6237.46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1611.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>